<commit_message>
final for phase 3
</commit_message>
<xml_diff>
--- a/graphs+excel_directory/generated_spreadsheet.xlsx
+++ b/graphs+excel_directory/generated_spreadsheet.xlsx
@@ -12,13 +12,14 @@
     <sheet name="simple_exponential_smoothing" sheetId="3" r:id="rId3"/>
     <sheet name="holt_trend_exp_smoothing" sheetId="4" r:id="rId4"/>
     <sheet name="winter_trendseason" sheetId="5" r:id="rId5"/>
+    <sheet name="Find_EOQ_cycle_inventory" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="28">
   <si>
     <t>Year</t>
   </si>
@@ -75,6 +76,33 @@
   </si>
   <si>
     <t>Seasonal Factor</t>
+  </si>
+  <si>
+    <t>Annual demand (Forecasted,cumulative)</t>
+  </si>
+  <si>
+    <t>Shipment cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Holding cost </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Material Cost </t>
+  </si>
+  <si>
+    <t>OPTIMAL LOT SIZE</t>
+  </si>
+  <si>
+    <t>Cycle Inventory</t>
+  </si>
+  <si>
+    <t>Number of Orders Per Year:</t>
+  </si>
+  <si>
+    <t>Replenishment time:</t>
+  </si>
+  <si>
+    <t>Average Flow time:</t>
   </si>
 </sst>
 </file>
@@ -3001,4 +3029,87 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>101532.9182272287</v>
+      </c>
+      <c r="B2">
+        <v>7500</v>
+      </c>
+      <c r="C2">
+        <v>0.1</v>
+      </c>
+      <c r="D2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>3902.555282642939</v>
+      </c>
+      <c r="B4">
+        <v>1951.277641321469</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>26.01703521761959</v>
+      </c>
+      <c r="B6">
+        <v>14.02926955154406</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>7.014634775772031</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>